<commit_message>
add some comment to preprocess
</commit_message>
<xml_diff>
--- a/Get_Properties_Notebook-WI/gp_start_folder/pyrd_atom_map.xlsx
+++ b/Get_Properties_Notebook-WI/gp_start_folder/pyrd_atom_map.xlsx
@@ -658,19 +658,19 @@
         <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8">

</xml_diff>

<commit_message>
matching the side alkyl chain as substructure
</commit_message>
<xml_diff>
--- a/Get_Properties_Notebook-WI/gp_start_folder/pyrd_atom_map.xlsx
+++ b/Get_Properties_Notebook-WI/gp_start_folder/pyrd_atom_map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="66">
   <si>
     <t>log_name</t>
   </si>
@@ -31,6 +31,12 @@
     <t>N1</t>
   </si>
   <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
     <t>C1</t>
   </si>
   <si>
@@ -151,9 +157,6 @@
     <t>C10</t>
   </si>
   <si>
-    <t>C6</t>
-  </si>
-  <si>
     <t>C8</t>
   </si>
   <si>
@@ -163,9 +166,6 @@
     <t>C11</t>
   </si>
   <si>
-    <t>C7</t>
-  </si>
-  <si>
     <t>C9</t>
   </si>
   <si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
   </si>
 </sst>
 </file>
@@ -566,13 +569,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,360 +597,444 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
         <v>54</v>
       </c>
       <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="H3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
         <v>54</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>50</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
         <v>54</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>54</v>
       </c>
       <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>46</v>
       </c>
-      <c r="H6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
       <c r="D7" t="s">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>54</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
         <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
         <v>54</v>
       </c>
       <c r="G9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F10" t="s">
         <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s">
         <v>54</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
         <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H12" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F13" t="s">
         <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H13" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
         <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s">
         <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="H14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
         <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
         <v>55</v>
@@ -958,16 +1045,22 @@
       <c r="H15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -979,18 +1072,24 @@
         <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H16" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -1005,18 +1104,24 @@
         <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -1031,27 +1136,33 @@
         <v>57</v>
       </c>
       <c r="G18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+        <v>5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F19" t="s">
         <v>55</v>
@@ -1062,16 +1173,22 @@
       <c r="H19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>3</v>
@@ -1083,27 +1200,33 @@
         <v>58</v>
       </c>
       <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
         <v>6</v>
       </c>
-      <c r="H20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" t="s">
+        <v>47</v>
+      </c>
+      <c r="J20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
         <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="s">
-        <v>49</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -1114,22 +1237,28 @@
       <c r="H21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F22" t="s">
         <v>60</v>
@@ -1140,22 +1269,28 @@
       <c r="H22" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" t="s">
+        <v>50</v>
+      </c>
+      <c r="J22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F23" t="s">
         <v>60</v>
@@ -1166,22 +1301,28 @@
       <c r="H23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" t="s">
+        <v>50</v>
+      </c>
+      <c r="J23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F24" t="s">
         <v>60</v>
@@ -1192,22 +1333,28 @@
       <c r="H24" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" t="s">
+        <v>50</v>
+      </c>
+      <c r="J24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F25" t="s">
         <v>60</v>
@@ -1218,22 +1365,28 @@
       <c r="H25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F26" t="s">
         <v>60</v>
@@ -1244,22 +1397,28 @@
       <c r="H26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F27" t="s">
         <v>60</v>
@@ -1270,22 +1429,28 @@
       <c r="H27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" t="s">
+        <v>50</v>
+      </c>
+      <c r="J27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F28" t="s">
         <v>60</v>
@@ -1296,22 +1461,28 @@
       <c r="H28" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="E29" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="F29" t="s">
         <v>60</v>
@@ -1322,16 +1493,22 @@
       <c r="H29" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" t="s">
+        <v>50</v>
+      </c>
+      <c r="J29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
         <v>50</v>
@@ -1343,44 +1520,56 @@
         <v>58</v>
       </c>
       <c r="G30" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H30" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" t="s">
+        <v>49</v>
+      </c>
+      <c r="J30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
         <v>61</v>
       </c>
       <c r="G31" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H31" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
         <v>2</v>
@@ -1389,24 +1578,30 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F32" t="s">
         <v>61</v>
       </c>
       <c r="G32" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="H32" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -1415,27 +1610,33 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F33" t="s">
         <v>61</v>
       </c>
       <c r="G33" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="H33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
         <v>52</v>
@@ -1452,16 +1653,22 @@
       <c r="H34" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34" t="s">
+        <v>65</v>
+      </c>
+      <c r="J34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
         <v>52</v>
@@ -1478,19 +1685,25 @@
       <c r="H35" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" t="s">
+        <v>65</v>
+      </c>
+      <c r="J35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E36" t="s">
         <v>2</v>
@@ -1499,27 +1712,33 @@
         <v>58</v>
       </c>
       <c r="G36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H36" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36" t="s">
+        <v>51</v>
+      </c>
+      <c r="J36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D37" t="s">
         <v>52</v>
       </c>
       <c r="E37" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F37" t="s">
         <v>58</v>
@@ -1528,21 +1747,27 @@
         <v>2</v>
       </c>
       <c r="H37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+        <v>46</v>
+      </c>
+      <c r="I37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="E38" t="s">
         <v>2</v>
@@ -1551,10 +1776,16 @@
         <v>58</v>
       </c>
       <c r="G38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H38" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="I38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix substructure matching issues
</commit_message>
<xml_diff>
--- a/Get_Properties_Notebook-WI/gp_start_folder/pyrd_atom_map.xlsx
+++ b/Get_Properties_Notebook-WI/gp_start_folder/pyrd_atom_map.xlsx
@@ -25,12 +25,12 @@
     <t>C4</t>
   </si>
   <si>
+    <t>N1</t>
+  </si>
+  <si>
     <t>C5</t>
   </si>
   <si>
-    <t>N1</t>
-  </si>
-  <si>
     <t>C6</t>
   </si>
   <si>
@@ -154,61 +154,61 @@
     <t>pyrd9_conf-1</t>
   </si>
   <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
     <t>C10</t>
   </si>
   <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>N7</t>
+  </si>
+  <si>
+    <t>N10</t>
+  </si>
+  <si>
+    <t>N11</t>
+  </si>
+  <si>
+    <t>N12</t>
+  </si>
+  <si>
+    <t>N3</t>
+  </si>
+  <si>
+    <t>N6</t>
+  </si>
+  <si>
+    <t>N5</t>
+  </si>
+  <si>
+    <t>N16</t>
+  </si>
+  <si>
+    <t>N15</t>
+  </si>
+  <si>
     <t>C8</t>
   </si>
   <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
     <t>C19</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C13</t>
-  </si>
-  <si>
-    <t>C14</t>
-  </si>
-  <si>
-    <t>N7</t>
-  </si>
-  <si>
-    <t>N10</t>
-  </si>
-  <si>
-    <t>N11</t>
-  </si>
-  <si>
-    <t>N12</t>
-  </si>
-  <si>
-    <t>N3</t>
-  </si>
-  <si>
-    <t>N6</t>
-  </si>
-  <si>
-    <t>N5</t>
-  </si>
-  <si>
-    <t>N16</t>
-  </si>
-  <si>
-    <t>N15</t>
-  </si>
-  <si>
-    <t>C16</t>
-  </si>
-  <si>
-    <t>C17</t>
   </si>
   <si>
     <t>C18</t>
@@ -612,28 +612,28 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
       </c>
       <c r="J2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -644,28 +644,28 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
         <v>2</v>
       </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -676,28 +676,28 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
         <v>2</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -708,28 +708,28 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
         <v>2</v>
       </c>
       <c r="J5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -740,28 +740,28 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
         <v>2</v>
       </c>
       <c r="J6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -772,28 +772,28 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I7" t="s">
         <v>2</v>
       </c>
       <c r="J7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -804,28 +804,28 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
       </c>
       <c r="J8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -836,28 +836,28 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I9" t="s">
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -868,28 +868,28 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -900,28 +900,28 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I11" t="s">
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -932,28 +932,28 @@
         <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I12" t="s">
         <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -964,28 +964,28 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I13" t="s">
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -996,28 +996,28 @@
         <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="H14" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="I14" t="s">
         <v>2</v>
       </c>
       <c r="J14" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1028,22 +1028,22 @@
         <v>22</v>
       </c>
       <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
         <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1</v>
       </c>
       <c r="I15" t="s">
         <v>2</v>
@@ -1060,22 +1060,22 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" t="s">
         <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" t="s">
-        <v>51</v>
       </c>
       <c r="I16" t="s">
         <v>2</v>
@@ -1092,25 +1092,25 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G17" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" t="s">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" t="s">
-        <v>2</v>
-      </c>
       <c r="I17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J17" t="s">
         <v>2</v>
@@ -1124,22 +1124,22 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>5</v>
       </c>
       <c r="H18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I18" t="s">
         <v>6</v>
@@ -1156,25 +1156,25 @@
         <v>26</v>
       </c>
       <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
         <v>1</v>
       </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" t="s">
-        <v>2</v>
-      </c>
       <c r="I19" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="J19" t="s">
         <v>1</v>
@@ -1188,25 +1188,25 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="G20" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I20" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="J20" t="s">
         <v>6</v>
@@ -1220,25 +1220,25 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
+      <c r="H21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>59</v>
-      </c>
-      <c r="G21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" t="s">
-        <v>1</v>
-      </c>
       <c r="I21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" t="s">
         <v>2</v>
@@ -1252,28 +1252,28 @@
         <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G22" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H22" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I22" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J22" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1284,28 +1284,28 @@
         <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H23" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J23" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1316,28 +1316,28 @@
         <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H24" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I24" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J24" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1348,28 +1348,28 @@
         <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G25" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H25" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J25" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1380,28 +1380,28 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G26" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H26" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I26" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J26" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1412,28 +1412,28 @@
         <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E27" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H27" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I27" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J27" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1444,28 +1444,28 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G28" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H28" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I28" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J28" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1476,28 +1476,28 @@
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="H29" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J29" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1511,25 +1511,25 @@
         <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="F30" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="H30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I30" t="s">
         <v>49</v>
       </c>
       <c r="J30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1540,25 +1540,25 @@
         <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" t="s">
         <v>6</v>
       </c>
-      <c r="F31" t="s">
-        <v>61</v>
-      </c>
       <c r="G31" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H31" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J31" t="s">
         <v>2</v>
@@ -1572,25 +1572,25 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H32" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J32" t="s">
         <v>2</v>
@@ -1604,25 +1604,25 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="G33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H33" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J33" t="s">
         <v>2</v>
@@ -1636,13 +1636,13 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F34" t="s">
         <v>62</v>
@@ -1657,7 +1657,7 @@
         <v>65</v>
       </c>
       <c r="J34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1668,13 +1668,13 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F35" t="s">
         <v>62</v>
@@ -1689,7 +1689,7 @@
         <v>65</v>
       </c>
       <c r="J35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1700,25 +1700,25 @@
         <v>43</v>
       </c>
       <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" t="s">
         <v>49</v>
       </c>
-      <c r="D36" t="s">
-        <v>46</v>
-      </c>
-      <c r="E36" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" t="s">
-        <v>58</v>
-      </c>
-      <c r="G36" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" t="s">
-        <v>52</v>
-      </c>
       <c r="I36" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J36" t="s">
         <v>49</v>
@@ -1732,25 +1732,25 @@
         <v>44</v>
       </c>
       <c r="C37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" t="s">
+        <v>47</v>
+      </c>
+      <c r="H37" t="s">
         <v>49</v>
       </c>
-      <c r="D37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" t="s">
-        <v>8</v>
-      </c>
-      <c r="F37" t="s">
-        <v>58</v>
-      </c>
-      <c r="G37" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" t="s">
-        <v>46</v>
-      </c>
       <c r="I37" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J37" t="s">
         <v>49</v>
@@ -1764,22 +1764,22 @@
         <v>45</v>
       </c>
       <c r="C38" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" t="s">
         <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" t="s">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" t="s">
-        <v>47</v>
       </c>
       <c r="I38" t="s">
         <v>7</v>

</xml_diff>